<commit_message>
updated for last version hopefullz
</commit_message>
<xml_diff>
--- a/logBookBFA_MA-19.xlsx
+++ b/logBookBFA_MA-19.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin.FONTANA\Documents\GitHub\MA-19-Domotique\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenan.AUGSBURGER\Documents\Github\MA-19\MA-19-Domotique\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641BA3A1-9DE3-4170-BD6F-5DD0B605864D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17670" windowHeight="8085"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -26,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
-    <t>Descritpion</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -50,40 +57,43 @@
     <t>Utilisations de différents matériel</t>
   </si>
   <si>
-    <t>Mise en place d'edomus</t>
-  </si>
-  <si>
-    <t>Reinstallation Raspberry pi et domoticz</t>
-  </si>
-  <si>
-    <t>Theorie cablage plus debut de la maquette</t>
-  </si>
-  <si>
-    <t>Maquette presque terminee, circuit 12v restant</t>
-  </si>
-  <si>
-    <t>Fin de la maquette sans qubino, debut de l'ajout du qubino</t>
-  </si>
-  <si>
     <t>Fin de la maquette avec qubino, Appairage des appareils z-wave</t>
   </si>
   <si>
-    <t>Ajout des appareils enocean et debut des scenarii</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Travail sur les scénarios</t>
   </si>
   <si>
     <t>Documentation et scénarios</t>
   </si>
   <si>
-    <t>Finalitation de la documentation</t>
+    <t>Mise en place d'Eedomus</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Réinstallation Raspberry pi et domoticz</t>
+  </si>
+  <si>
+    <t>Théorie câblage plus début de la maquette</t>
+  </si>
+  <si>
+    <t>Maquette presque terminée, circuit 12v restant</t>
+  </si>
+  <si>
+    <t>Fin de la maquette sans qubino, début de l'ajout du qubino</t>
+  </si>
+  <si>
+    <t>Ajout des appareils enocean et début des scénarios</t>
+  </si>
+  <si>
+    <t>Finalisation de la documentation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -195,17 +205,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F100" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:F100"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau2" displayName="Tableau2" ref="A1:F100" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:F100" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
-    <tableColumn id="3" name="Descritpion" dataDxfId="5"/>
-    <tableColumn id="5" name="Date" dataDxfId="4"/>
-    <tableColumn id="6" name="Heure de début" dataDxfId="3"/>
-    <tableColumn id="7" name="Heure de fin" dataDxfId="2"/>
-    <tableColumn id="8" name="Temps" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Date" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Heure de début" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Heure de fin" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Temps" dataDxfId="1">
       <calculatedColumnFormula>Tableau2[[#This Row],[Heure de fin]]-Tableau2[[#This Row],[Heure de début]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Sources" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Sources" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -473,14 +483,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="3" customWidth="1"/>
@@ -492,27 +502,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="6">
         <v>44236</v>
@@ -530,7 +540,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="6">
         <v>44237</v>
@@ -548,7 +558,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6">
         <v>44243</v>
@@ -566,7 +576,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="6">
         <v>44244</v>
@@ -584,7 +594,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" s="6">
         <v>44257</v>
@@ -602,7 +612,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" s="6">
         <v>44258</v>
@@ -620,7 +630,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B8" s="6">
         <v>44266</v>
@@ -638,7 +648,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B9" s="6">
         <v>44271</v>
@@ -656,7 +666,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10" s="6">
         <v>44272</v>
@@ -674,7 +684,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B11" s="6">
         <v>44278</v>
@@ -692,7 +702,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B12" s="6">
         <v>44279</v>
@@ -710,7 +720,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B13" s="6">
         <v>44285</v>
@@ -728,7 +738,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B14" s="6">
         <v>44286</v>

</xml_diff>